<commit_message>
Test Menu part 2
-Update Log Replaced with  Update Data
-Update Data can update Report Data
-Update Data can update Items
-Test App Data modified
-Adding New Items test success
-UI package added
-Get Index Case 1(Checking against Id) now has a possible fail case (if I actually have to use it)
-Add new Item is now removed
-Create New Item function finally completed
-Numerical only entries are now fully operational and work as intended
-tempSale & tempIndex Removed
-Update Data fully implemented(I think)
</commit_message>
<xml_diff>
--- a/TestAppData.xlsx
+++ b/TestAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redst\MobileApp\MomApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1B9F92-690C-47C6-87BD-3C30AC7AB3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A6BA3F-675A-4DF7-A29A-42CB4E13E9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>1s</t>
+  </si>
+  <si>
+    <t>Golden_Wind</t>
   </si>
 </sst>
 </file>
@@ -475,16 +481,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA678083-25DE-43B7-8E8B-3CB625356D8C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246A95FA-0848-4B0B-AFED-CA92ACC4E6CD}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -518,6 +527,26 @@
       <c r="D2" s="3">
         <v>0</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>13000006057</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>15.25</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
@@ -530,11 +559,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53E1FFE-83F7-4AE4-881F-EAFC4DFEE633}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,13 +630,33 @@
         <v>44504.407790594174</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A68ABEF-E54E-4A0D-BC1E-CB845EFCF729}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC96724E-D010-4FD6-91E3-11EAF160C917}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -653,10 +702,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046BBFBE-75A7-4327-81AD-6438445D90ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B2BABB-9526-4539-AE90-5681BABA19A9}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bug fix and new addition
-Graphing Server seperated from graphing
-Graphing module
-Formatting for dates adjusted YYYY/MM/DD
-Get All Data Function
-Shopping cart bug kind of patched
-Packaging tool added
-Graphing customization in progress
-Place holder bars replaced
-Server testing started
</commit_message>
<xml_diff>
--- a/TestAppData.xlsx
+++ b/TestAppData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView windowHeight="9360" windowWidth="18000" xWindow="2640" yWindow="690"/>
+    <workbookView windowHeight="13140" windowWidth="24240" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Items" sheetId="1" relationships:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Revenue</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -72,16 +69,40 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Frogs</t>
-  </si>
-  <si>
-    <t>Who</t>
-  </si>
-  <si>
     <t>Velvet</t>
   </si>
   <si>
-    <t>Working</t>
+    <t>The_World</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Retarded</t>
+  </si>
+  <si>
+    <t>Memories</t>
+  </si>
+  <si>
+    <t>Piano_Book</t>
+  </si>
+  <si>
+    <t>Index_Cards</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>Render</t>
   </si>
 </sst>
 </file>
@@ -132,13 +153,48 @@
         <bgColor auto="true"/>
       </patternFill>
     </fill>
-    <fill/>
-    <fill/>
-    <fill/>
-    <fill/>
-    <fill/>
-    <fill/>
-    <fill/>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor auto="true"/>
+        <bgColor auto="true"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor auto="true"/>
+        <bgColor auto="true"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor auto="true"/>
+        <bgColor auto="true"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor auto="true"/>
+        <bgColor auto="true"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor auto="true"/>
+        <bgColor auto="true"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor auto="true"/>
+        <bgColor auto="true"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor auto="true"/>
+        <bgColor auto="true"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -231,27 +287,13 @@
     <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="2" fillId="3" fontId="0" numFmtId="22" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="22" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="4" fillId="5" fontId="0" numFmtId="22" xfId="0">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="5" fillId="6" fontId="0" numFmtId="22" xfId="0">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="6" fillId="7" fontId="0" numFmtId="22" xfId="0">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="7" fillId="8" fontId="0" numFmtId="22" xfId="0">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="8" fillId="9" fontId="0" numFmtId="22" xfId="0">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="9" fillId="10" fontId="0" numFmtId="22" xfId="0">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="10" fillId="11" fontId="0" numFmtId="22" xfId="0">
-      <alignment/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="4" fillId="5" fontId="0" numFmtId="22" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="5" fillId="6" fontId="0" numFmtId="22" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="6" fillId="7" fontId="0" numFmtId="22" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="7" fillId="8" fontId="0" numFmtId="22" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="8" fillId="9" fontId="0" numFmtId="22" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="9" fillId="10" fontId="0" numFmtId="22" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="10" fillId="11" fontId="0" numFmtId="22" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -566,15 +608,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="41.42578125"/>
     <col bestFit="true" collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="5.42578125"/>
     <col bestFit="true" collapsed="false" customWidth="true" hidden="false" max="5" min="5" style="0" width="9.5703125"/>
   </cols>
@@ -609,13 +652,16 @@
       <c r="D2" s="3">
         <v>0</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
         <v>786936732658</v>
       </c>
-      <c r="B3" s="7" t="str">
-        <v>The_World</v>
+      <c r="B3" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -631,8 +677,8 @@
       <c r="A4">
         <v>725272730706</v>
       </c>
-      <c r="B4" t="str">
-        <v>Red</v>
+      <c r="B4" t="s">
+        <v>14</v>
       </c>
       <c r="C4">
         <v>33</v>
@@ -649,7 +695,7 @@
         <v>28400589895</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -665,8 +711,8 @@
       <c r="A6">
         <v>13000006057</v>
       </c>
-      <c r="B6" t="str">
-        <v>Retarded</v>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -682,8 +728,8 @@
       <c r="A7">
         <v>737452918903</v>
       </c>
-      <c r="B7" t="str">
-        <v>Memories</v>
+      <c r="B7" t="s">
+        <v>16</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -695,12 +741,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>674398202423</v>
       </c>
-      <c r="B8" t="str">
-        <v>Piano_Book</v>
+      <c r="B8" t="s">
+        <v>17</v>
       </c>
       <c r="C8">
         <v>43</v>
@@ -712,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>490810512013</v>
       </c>
@@ -720,10 +766,10 @@
         <v>Index_Cards</v>
       </c>
       <c r="C9">
-        <v>10.54</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -735,7 +781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE2A69D-CD5A-4926-9A93-857C98396B1C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C7EE5A-33BE-430A-9E01-648D4595B43F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -766,7 +812,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -812,7 +858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59E82D3-2C71-49E3-BDD4-1E525F4529C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDCF3F2-4DED-42BC-9358-E774FDD51861}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -834,7 +880,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -849,7 +895,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -858,19 +904,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B82F8B34-DFCF-4AD9-8CB6-6CDF95B44E42}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="true" collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="10.7109375"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -887,12 +933,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>13000006057</v>
       </c>
-      <c r="B2" s="1" t="str">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -901,15 +947,15 @@
         <v>1</v>
       </c>
       <c r="E2" s="8">
-        <v>44525.71917643866</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>44525.719176438659</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13000006057</v>
       </c>
-      <c r="B3" t="str">
-        <v>red</v>
+      <c r="B3" t="s">
+        <v>20</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -921,12 +967,12 @@
         <v>44525.719464839116</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13000006057</v>
       </c>
-      <c r="B4" t="str">
-        <v>4</v>
+      <c r="B4" t="s">
+        <v>21</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -938,12 +984,12 @@
         <v>44525.719869876615</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13000006057</v>
       </c>
-      <c r="B5" t="str">
-        <v>Same</v>
+      <c r="B5" t="s">
+        <v>22</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -952,15 +998,15 @@
         <v>1</v>
       </c>
       <c r="E5" s="11">
-        <v>44525.72240384563</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>44525.722403845633</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13000006057</v>
       </c>
-      <c r="B6" t="str">
-        <v>Cost</v>
+      <c r="B6" t="s">
+        <v>4</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -972,12 +1018,12 @@
         <v>44525.723437086286</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>13000006057</v>
       </c>
-      <c r="B7" t="str">
-        <v>Render</v>
+      <c r="B7" t="s">
+        <v>23</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -986,15 +1032,15 @@
         <v>2</v>
       </c>
       <c r="E7" s="13">
-        <v>44526.41935156452</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>44526.419351564517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>13000006057</v>
       </c>
-      <c r="B8" t="str">
-        <v>Retarded</v>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1003,10 +1049,10 @@
         <v>2</v>
       </c>
       <c r="E8" s="14">
-        <v>44526.42054798802</v>
+        <v>44526.420547988018</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>